<commit_message>
Started organized analyses file, started to work with compound classes
</commit_message>
<xml_diff>
--- a/Scent_Meta.xlsx
+++ b/Scent_Meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineeisen/github/oenothera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC1758F-EBA8-4145-B9DB-D14991D91EA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD791D5-807F-1A4C-95B6-3618E02E7B04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="8780" windowWidth="26440" windowHeight="15440" xr2:uid="{79BE3B78-3A96-E146-9198-FC83B2C3D2DA}"/>
+    <workbookView xWindow="10740" yWindow="6340" windowWidth="26440" windowHeight="15440" xr2:uid="{79BE3B78-3A96-E146-9198-FC83B2C3D2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="290">
   <si>
     <t>Population</t>
   </si>
@@ -553,6 +553,348 @@
   </si>
   <si>
     <t>Samp.rm5-29-B</t>
+  </si>
+  <si>
+    <t>Samp.rm3-4-B</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>rm2-1</t>
+  </si>
+  <si>
+    <t>Samp.rm2-1-A</t>
+  </si>
+  <si>
+    <t>rm2-3</t>
+  </si>
+  <si>
+    <t>Samp.rm2-3-A</t>
+  </si>
+  <si>
+    <t>rm2-5</t>
+  </si>
+  <si>
+    <t>Samp.rm2-5-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-5-B</t>
+  </si>
+  <si>
+    <t>rm2-6</t>
+  </si>
+  <si>
+    <t>Samp.rm2-6-A</t>
+  </si>
+  <si>
+    <t>rm2-7</t>
+  </si>
+  <si>
+    <t>Samp.rm2-7-A</t>
+  </si>
+  <si>
+    <t>rm2-8</t>
+  </si>
+  <si>
+    <t>Samp.rm2-8-A</t>
+  </si>
+  <si>
+    <t>rm2-9</t>
+  </si>
+  <si>
+    <t>Samp.rm2-9-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-9-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-9-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-9-D</t>
+  </si>
+  <si>
+    <t>rm2-11</t>
+  </si>
+  <si>
+    <t>Samp.rm2-11-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-11-B</t>
+  </si>
+  <si>
+    <t>rm2-11a</t>
+  </si>
+  <si>
+    <t>Samp.rm2-11-C</t>
+  </si>
+  <si>
+    <t>rm2-11b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-11-D</t>
+  </si>
+  <si>
+    <t>rm2-13</t>
+  </si>
+  <si>
+    <t>Samp.rm2-13-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-13-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-13-C</t>
+  </si>
+  <si>
+    <t>rm2-13b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-13-D</t>
+  </si>
+  <si>
+    <t>rm2-15</t>
+  </si>
+  <si>
+    <t>Samp.rm2-15-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-15-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-15-C</t>
+  </si>
+  <si>
+    <t>rm2-16</t>
+  </si>
+  <si>
+    <t>Samp.rm2-16-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-16-B</t>
+  </si>
+  <si>
+    <t>mr2-16</t>
+  </si>
+  <si>
+    <t>Samp.mr2-16-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-16-D</t>
+  </si>
+  <si>
+    <t>rm2-17</t>
+  </si>
+  <si>
+    <t>Samp.rm2-17-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-17-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-17-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-17-D</t>
+  </si>
+  <si>
+    <t>rm2-18</t>
+  </si>
+  <si>
+    <t>Samp.rm2-18-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-18-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-18-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-18-D</t>
+  </si>
+  <si>
+    <t>rm2-19</t>
+  </si>
+  <si>
+    <t>Samp.rm2-19-A</t>
+  </si>
+  <si>
+    <t>rm2-20</t>
+  </si>
+  <si>
+    <t>Samp.rm2-20-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-20-B</t>
+  </si>
+  <si>
+    <t>rm2-21</t>
+  </si>
+  <si>
+    <t>Samp.rm2-21-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-21-B</t>
+  </si>
+  <si>
+    <t>rm2-23b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-23-A</t>
+  </si>
+  <si>
+    <t>rm2-23</t>
+  </si>
+  <si>
+    <t>Samp.rm2-23-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-23-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-23-D</t>
+  </si>
+  <si>
+    <t>rm2-25</t>
+  </si>
+  <si>
+    <t>Samp.rm2-25-A</t>
+  </si>
+  <si>
+    <t>rm2-25b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-25-B</t>
+  </si>
+  <si>
+    <t>rm2-25-1</t>
+  </si>
+  <si>
+    <t>Samp.rm2-25-C</t>
+  </si>
+  <si>
+    <t>rm2-25-2</t>
+  </si>
+  <si>
+    <t>Samp.rm2-25-D</t>
+  </si>
+  <si>
+    <t>rm2-26</t>
+  </si>
+  <si>
+    <t>Samp.rm2-26-A</t>
+  </si>
+  <si>
+    <t>rm2-27-1</t>
+  </si>
+  <si>
+    <t>Samp.rm2-27-A</t>
+  </si>
+  <si>
+    <t>rm2-27</t>
+  </si>
+  <si>
+    <t>rm2-27-2</t>
+  </si>
+  <si>
+    <t>Samp.rm2-27-B</t>
+  </si>
+  <si>
+    <t>rm2-28</t>
+  </si>
+  <si>
+    <t>Samp.rm2-28-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-28-B</t>
+  </si>
+  <si>
+    <t>rm2-28-1</t>
+  </si>
+  <si>
+    <t>Samp.rm2-28-C</t>
+  </si>
+  <si>
+    <t>rm2-28-2</t>
+  </si>
+  <si>
+    <t>Samp.rm2-28-D</t>
+  </si>
+  <si>
+    <t>Samp.rm2-28-E</t>
+  </si>
+  <si>
+    <t>rm2-29</t>
+  </si>
+  <si>
+    <t>Samp.rm2-29-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-29-B</t>
+  </si>
+  <si>
+    <t>rm2-30</t>
+  </si>
+  <si>
+    <t>Samp.rm2-30-A</t>
+  </si>
+  <si>
+    <t>rm2-31</t>
+  </si>
+  <si>
+    <t>Samp.rm2-31-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-31-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-31-C</t>
+  </si>
+  <si>
+    <t>rm2-32</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-A</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-C</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-D</t>
+  </si>
+  <si>
+    <t>rm2-32b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-E</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-F</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-G</t>
+  </si>
+  <si>
+    <t>Samp.rm2-32-H</t>
+  </si>
+  <si>
+    <t>rm2-33</t>
+  </si>
+  <si>
+    <t>Samp.rm2-33-A</t>
+  </si>
+  <si>
+    <t>rm2-33b</t>
+  </si>
+  <si>
+    <t>Samp.rm2-33-B</t>
+  </si>
+  <si>
+    <t>Samp.rm2-33-C</t>
   </si>
 </sst>
 </file>
@@ -562,7 +904,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -596,8 +938,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,6 +983,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -641,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -678,6 +1081,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -994,15 +1466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4119944B-C687-9141-8416-0EE455816FF6}">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1562,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1606,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1650,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1694,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1738,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1782,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1826,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +1870,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1878,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
@@ -1442,7 +1914,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1958,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1530,7 +2002,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1574,7 +2046,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1618,7 +2090,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +2134,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1706,7 +2178,7 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +2222,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1794,7 +2266,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -1838,7 +2310,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +2354,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +2398,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1970,7 +2442,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -2014,7 +2486,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2530,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +2574,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2146,7 +2618,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -2190,7 +2662,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -2234,7 +2706,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2750,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2322,7 +2794,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2838,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -2410,7 +2882,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2926,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -2498,7 +2970,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2542,7 +3014,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
@@ -2586,7 +3058,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -2630,7 +3102,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -2674,7 +3146,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -2718,7 +3190,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +3234,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
@@ -2806,7 +3278,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +3322,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
@@ -2894,7 +3366,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -2938,7 +3410,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -2982,7 +3454,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -3026,7 +3498,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -3070,7 +3542,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
@@ -3114,7 +3586,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
@@ -3158,7 +3630,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
@@ -3202,7 +3674,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
@@ -3246,7 +3718,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -3290,7 +3762,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
         <v>39</v>
       </c>
@@ -3334,7 +3806,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -3378,7 +3850,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
@@ -3422,7 +3894,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -3466,7 +3938,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
@@ -3510,7 +3982,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" s="1" t="s">
         <v>39</v>
       </c>
@@ -3554,7 +4026,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -3598,7 +4070,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="A60" s="1" t="s">
         <v>39</v>
       </c>
@@ -3642,7 +4114,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14">
       <c r="A61" s="1" t="s">
         <v>39</v>
       </c>
@@ -3686,7 +4158,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -3730,7 +4202,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14">
       <c r="A63" s="1" t="s">
         <v>45</v>
       </c>
@@ -3774,7 +4246,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14">
       <c r="A64" s="1" t="s">
         <v>45</v>
       </c>
@@ -3818,7 +4290,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>45</v>
       </c>
@@ -3862,7 +4334,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
@@ -3906,7 +4378,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>45</v>
       </c>
@@ -3950,7 +4422,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
@@ -3994,7 +4466,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
@@ -4038,7 +4510,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
@@ -4082,7 +4554,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>45</v>
       </c>
@@ -4126,7 +4598,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>45</v>
       </c>
@@ -4170,7 +4642,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>45</v>
       </c>
@@ -4214,7 +4686,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14">
       <c r="A74" s="1" t="s">
         <v>45</v>
       </c>
@@ -4258,7 +4730,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14">
       <c r="A75" s="1" t="s">
         <v>45</v>
       </c>
@@ -4302,7 +4774,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14">
       <c r="A76" s="1" t="s">
         <v>45</v>
       </c>
@@ -4346,7 +4818,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14">
       <c r="A77" s="1" t="s">
         <v>45</v>
       </c>
@@ -4390,7 +4862,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14">
       <c r="A78" s="1" t="s">
         <v>45</v>
       </c>
@@ -4434,7 +4906,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14">
       <c r="A79" s="1" t="s">
         <v>45</v>
       </c>
@@ -4478,7 +4950,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14">
       <c r="A80" s="1" t="s">
         <v>45</v>
       </c>
@@ -4522,7 +4994,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14">
       <c r="A81" s="1" t="s">
         <v>45</v>
       </c>
@@ -4566,7 +5038,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14">
       <c r="A82" s="1" t="s">
         <v>45</v>
       </c>
@@ -4610,7 +5082,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14">
       <c r="A83" s="1" t="s">
         <v>45</v>
       </c>
@@ -4654,7 +5126,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -4698,7 +5170,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14">
       <c r="A85" s="1" t="s">
         <v>45</v>
       </c>
@@ -4742,7 +5214,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14">
       <c r="A86" s="1" t="s">
         <v>45</v>
       </c>
@@ -4786,7 +5258,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14">
       <c r="A87" s="1" t="s">
         <v>61</v>
       </c>
@@ -4830,7 +5302,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14">
       <c r="A88" s="1" t="s">
         <v>61</v>
       </c>
@@ -4874,7 +5346,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14">
       <c r="A89" s="1" t="s">
         <v>61</v>
       </c>
@@ -4918,7 +5390,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14">
       <c r="A90" s="1" t="s">
         <v>61</v>
       </c>
@@ -4962,7 +5434,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14">
       <c r="A91" s="1" t="s">
         <v>61</v>
       </c>
@@ -5006,7 +5478,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14">
       <c r="A92" s="1" t="s">
         <v>61</v>
       </c>
@@ -5050,7 +5522,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14">
       <c r="A93" s="1" t="s">
         <v>61</v>
       </c>
@@ -5094,7 +5566,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14">
       <c r="A94" s="1" t="s">
         <v>61</v>
       </c>
@@ -5138,7 +5610,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14">
       <c r="A95" s="1" t="s">
         <v>61</v>
       </c>
@@ -5155,13 +5627,13 @@
         <v>1</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G95" s="3">
-        <v>40015</v>
+        <v>39989</v>
       </c>
       <c r="H95" s="10">
-        <v>30812928</v>
+        <v>3752719</v>
       </c>
       <c r="I95">
         <v>23</v>
@@ -5176,13 +5648,13 @@
         <v>1</v>
       </c>
       <c r="M95" s="12">
-        <v>3.01</v>
+        <v>3.15</v>
       </c>
       <c r="N95" s="12">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" s="1" t="s">
         <v>61</v>
       </c>
@@ -5199,13 +5671,13 @@
         <v>2</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G96" s="3">
-        <v>39989</v>
+        <v>40015</v>
       </c>
       <c r="H96" s="10">
-        <v>3752719</v>
+        <v>30812928</v>
       </c>
       <c r="I96">
         <v>23</v>
@@ -5220,13 +5692,13 @@
         <v>1</v>
       </c>
       <c r="M96" s="12">
-        <v>3.15</v>
+        <v>3.01</v>
       </c>
       <c r="N96" s="12">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="1" t="s">
         <v>61</v>
       </c>
@@ -5270,7 +5742,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14">
       <c r="A98" s="1" t="s">
         <v>61</v>
       </c>
@@ -5314,7 +5786,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14">
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
@@ -5355,6 +5827,3174 @@
         <v>3.07</v>
       </c>
       <c r="N99" s="12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="A100" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G100" s="23">
+        <v>39989</v>
+      </c>
+      <c r="H100" s="10">
+        <v>6741483</v>
+      </c>
+      <c r="I100">
+        <v>23</v>
+      </c>
+      <c r="J100">
+        <v>55</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100" s="42">
+        <v>2.1</v>
+      </c>
+      <c r="N100" s="42">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" s="23">
+        <v>39989</v>
+      </c>
+      <c r="H101" s="10">
+        <v>5886478</v>
+      </c>
+      <c r="I101">
+        <v>23</v>
+      </c>
+      <c r="J101">
+        <v>55</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+      <c r="M101" s="42">
+        <v>2.83</v>
+      </c>
+      <c r="N101" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" s="25">
+        <v>39980</v>
+      </c>
+      <c r="H102" s="10">
+        <v>5789065</v>
+      </c>
+      <c r="I102">
+        <v>23</v>
+      </c>
+      <c r="J102">
+        <v>55</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>1</v>
+      </c>
+      <c r="M102" s="42">
+        <v>1.98</v>
+      </c>
+      <c r="N102" s="42">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D103" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E103" s="1">
+        <v>2</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="25">
+        <v>39989</v>
+      </c>
+      <c r="H103" s="10">
+        <v>4875529</v>
+      </c>
+      <c r="I103">
+        <v>23</v>
+      </c>
+      <c r="J103">
+        <v>55</v>
+      </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103">
+        <v>1</v>
+      </c>
+      <c r="M103" s="42">
+        <v>2.13</v>
+      </c>
+      <c r="N103" s="42">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D104" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G104" s="23">
+        <v>39989</v>
+      </c>
+      <c r="H104" s="10">
+        <v>4697269</v>
+      </c>
+      <c r="I104">
+        <v>23</v>
+      </c>
+      <c r="J104">
+        <v>55</v>
+      </c>
+      <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="L104">
+        <v>1</v>
+      </c>
+      <c r="M104" s="42">
+        <v>1.63</v>
+      </c>
+      <c r="N104" s="42">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D105" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105" s="23">
+        <v>39979</v>
+      </c>
+      <c r="H105" s="10">
+        <v>5742990</v>
+      </c>
+      <c r="I105">
+        <v>23</v>
+      </c>
+      <c r="J105">
+        <v>55</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105">
+        <v>1</v>
+      </c>
+      <c r="M105" s="42">
+        <v>2.21</v>
+      </c>
+      <c r="N105" s="42">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G106" s="23">
+        <v>39989</v>
+      </c>
+      <c r="H106" s="10">
+        <v>6801250</v>
+      </c>
+      <c r="I106">
+        <v>23</v>
+      </c>
+      <c r="J106">
+        <v>55</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106">
+        <v>1</v>
+      </c>
+      <c r="M106" s="42">
+        <v>2.72</v>
+      </c>
+      <c r="N106" s="42">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B107" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="D107" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E107" s="1">
+        <v>1</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G107" s="25">
+        <v>39965</v>
+      </c>
+      <c r="H107" s="10">
+        <v>5338464</v>
+      </c>
+      <c r="I107">
+        <v>23</v>
+      </c>
+      <c r="J107">
+        <v>55</v>
+      </c>
+      <c r="K107">
+        <v>1</v>
+      </c>
+      <c r="L107">
+        <v>1</v>
+      </c>
+      <c r="M107" s="42">
+        <v>3.3</v>
+      </c>
+      <c r="N107" s="42">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="A108" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B108" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E108" s="1">
+        <v>2</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G108" s="25">
+        <v>39972</v>
+      </c>
+      <c r="H108" s="10">
+        <v>3224606</v>
+      </c>
+      <c r="I108">
+        <v>23</v>
+      </c>
+      <c r="J108">
+        <v>55</v>
+      </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
+        <v>1</v>
+      </c>
+      <c r="M108" s="42">
+        <v>2.81</v>
+      </c>
+      <c r="N108" s="42">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E109" s="1">
+        <v>3</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G109" s="25">
+        <v>39988</v>
+      </c>
+      <c r="H109" s="10">
+        <v>6525741</v>
+      </c>
+      <c r="I109">
+        <v>23</v>
+      </c>
+      <c r="J109">
+        <v>55</v>
+      </c>
+      <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109">
+        <v>1</v>
+      </c>
+      <c r="M109" s="42">
+        <v>2.87</v>
+      </c>
+      <c r="N109" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B110" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E110" s="1">
+        <v>4</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" s="25">
+        <v>39989</v>
+      </c>
+      <c r="H110" s="10">
+        <v>6594052</v>
+      </c>
+      <c r="I110">
+        <v>23</v>
+      </c>
+      <c r="J110">
+        <v>55</v>
+      </c>
+      <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110">
+        <v>1</v>
+      </c>
+      <c r="M110" s="42">
+        <v>2.91</v>
+      </c>
+      <c r="N110" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="A111" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B111" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G111" s="27">
+        <v>39972</v>
+      </c>
+      <c r="H111" s="10">
+        <v>2973401</v>
+      </c>
+      <c r="I111">
+        <v>23</v>
+      </c>
+      <c r="J111">
+        <v>55</v>
+      </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111">
+        <v>1</v>
+      </c>
+      <c r="M111" s="42">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="N111" s="42">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="A112" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B112" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C112" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D112" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E112" s="1">
+        <v>2</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G112" s="27">
+        <v>39980</v>
+      </c>
+      <c r="H112" s="10">
+        <v>6641677</v>
+      </c>
+      <c r="I112">
+        <v>23</v>
+      </c>
+      <c r="J112">
+        <v>55</v>
+      </c>
+      <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="L112">
+        <v>1</v>
+      </c>
+      <c r="M112" s="42">
+        <v>2.64</v>
+      </c>
+      <c r="N112" s="42">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B113" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D113" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E113" s="1">
+        <v>3</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G113" s="27">
+        <v>39981</v>
+      </c>
+      <c r="H113" s="10">
+        <v>6029157</v>
+      </c>
+      <c r="I113">
+        <v>23</v>
+      </c>
+      <c r="J113">
+        <v>55</v>
+      </c>
+      <c r="K113">
+        <v>1</v>
+      </c>
+      <c r="L113">
+        <v>1</v>
+      </c>
+      <c r="M113" s="42">
+        <v>2.91</v>
+      </c>
+      <c r="N113" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E114" s="1">
+        <v>4</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" s="27">
+        <v>39981</v>
+      </c>
+      <c r="H114" s="10">
+        <v>6187466</v>
+      </c>
+      <c r="I114">
+        <v>23</v>
+      </c>
+      <c r="J114">
+        <v>55</v>
+      </c>
+      <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <v>1</v>
+      </c>
+      <c r="M114" s="42">
+        <v>2.97</v>
+      </c>
+      <c r="N114" s="42">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B115" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D115" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E115" s="1">
+        <v>1</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G115" s="29">
+        <v>39965</v>
+      </c>
+      <c r="H115" s="10">
+        <v>8201924</v>
+      </c>
+      <c r="I115">
+        <v>23</v>
+      </c>
+      <c r="J115">
+        <v>55</v>
+      </c>
+      <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115">
+        <v>1</v>
+      </c>
+      <c r="M115" s="42">
+        <v>2.39</v>
+      </c>
+      <c r="N115" s="42">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="A116" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D116" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E116" s="1">
+        <v>2</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G116" s="29">
+        <v>39973</v>
+      </c>
+      <c r="H116" s="10">
+        <v>3520042</v>
+      </c>
+      <c r="I116">
+        <v>23</v>
+      </c>
+      <c r="J116">
+        <v>55</v>
+      </c>
+      <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <v>1</v>
+      </c>
+      <c r="M116" s="42">
+        <v>2.75</v>
+      </c>
+      <c r="N116" s="42">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="A117" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C117" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D117" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E117" s="1">
+        <v>3</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G117" s="29">
+        <v>39986</v>
+      </c>
+      <c r="H117" s="10">
+        <v>6769325</v>
+      </c>
+      <c r="I117">
+        <v>23</v>
+      </c>
+      <c r="J117">
+        <v>55</v>
+      </c>
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117" s="43">
+        <v>2.8</v>
+      </c>
+      <c r="N117" s="43">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="A118" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E118" s="1">
+        <v>4</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" s="29">
+        <v>39986</v>
+      </c>
+      <c r="H118" s="10">
+        <v>6714236</v>
+      </c>
+      <c r="I118">
+        <v>23</v>
+      </c>
+      <c r="J118">
+        <v>55</v>
+      </c>
+      <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="L118">
+        <v>1</v>
+      </c>
+      <c r="M118" s="42">
+        <v>3.25</v>
+      </c>
+      <c r="N118" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="A119" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B119" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="C119" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D119" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G119" s="31">
+        <v>39960</v>
+      </c>
+      <c r="H119" s="10">
+        <v>4046641</v>
+      </c>
+      <c r="I119">
+        <v>23</v>
+      </c>
+      <c r="J119">
+        <v>55</v>
+      </c>
+      <c r="K119">
+        <v>1</v>
+      </c>
+      <c r="L119">
+        <v>1</v>
+      </c>
+      <c r="M119" s="42">
+        <v>2.42</v>
+      </c>
+      <c r="N119" s="43">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="A120" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B120" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="E120" s="1">
+        <v>2</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="31">
+        <v>39981</v>
+      </c>
+      <c r="H120" s="10">
+        <v>6861636</v>
+      </c>
+      <c r="I120">
+        <v>23</v>
+      </c>
+      <c r="J120">
+        <v>55</v>
+      </c>
+      <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="L120">
+        <v>1</v>
+      </c>
+      <c r="M120" s="42">
+        <v>2.62</v>
+      </c>
+      <c r="N120" s="42">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="A121" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="C121" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="E121" s="1">
+        <v>3</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" s="31">
+        <v>39992</v>
+      </c>
+      <c r="H121" s="16">
+        <v>5049479</v>
+      </c>
+      <c r="I121">
+        <v>23</v>
+      </c>
+      <c r="J121">
+        <v>55</v>
+      </c>
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>1</v>
+      </c>
+      <c r="M121" s="42">
+        <v>2.33</v>
+      </c>
+      <c r="N121" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="A122" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B122" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D122" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G122" s="33">
+        <v>39954</v>
+      </c>
+      <c r="H122" s="10">
+        <v>3613748</v>
+      </c>
+      <c r="I122">
+        <v>23</v>
+      </c>
+      <c r="J122">
+        <v>55</v>
+      </c>
+      <c r="K122">
+        <v>1</v>
+      </c>
+      <c r="L122">
+        <v>1</v>
+      </c>
+      <c r="M122" s="42">
+        <v>2.25</v>
+      </c>
+      <c r="N122" s="43">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="A123" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B123" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D123" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E123" s="1">
+        <v>2</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G123" s="33">
+        <v>39965</v>
+      </c>
+      <c r="H123" s="10">
+        <v>8551782</v>
+      </c>
+      <c r="I123">
+        <v>23</v>
+      </c>
+      <c r="J123">
+        <v>55</v>
+      </c>
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
+        <v>1</v>
+      </c>
+      <c r="M123" s="42">
+        <v>2.23</v>
+      </c>
+      <c r="N123" s="42">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="A124" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C124" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D124" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="E124" s="1">
+        <v>3</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G124" s="33">
+        <v>39986</v>
+      </c>
+      <c r="H124" s="10">
+        <v>6207631</v>
+      </c>
+      <c r="I124">
+        <v>23</v>
+      </c>
+      <c r="J124">
+        <v>55</v>
+      </c>
+      <c r="K124">
+        <v>1</v>
+      </c>
+      <c r="L124">
+        <v>1</v>
+      </c>
+      <c r="M124" s="42">
+        <v>2.35</v>
+      </c>
+      <c r="N124" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="A125" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B125" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C125" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="D125" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E125" s="1">
+        <v>4</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G125" s="33">
+        <v>39993</v>
+      </c>
+      <c r="H125" s="10">
+        <v>4736910</v>
+      </c>
+      <c r="I125">
+        <v>23</v>
+      </c>
+      <c r="J125">
+        <v>55</v>
+      </c>
+      <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
+        <v>1</v>
+      </c>
+      <c r="M125" s="42">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="N125" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B126" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D126" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E126" s="1">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G126" s="25">
+        <v>39973</v>
+      </c>
+      <c r="H126" s="10">
+        <v>7357217</v>
+      </c>
+      <c r="I126">
+        <v>23</v>
+      </c>
+      <c r="J126">
+        <v>55</v>
+      </c>
+      <c r="K126">
+        <v>1</v>
+      </c>
+      <c r="L126">
+        <v>1</v>
+      </c>
+      <c r="M126" s="42">
+        <v>2.23</v>
+      </c>
+      <c r="N126" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B127" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D127" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E127" s="1">
+        <v>2</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G127" s="25">
+        <v>39986</v>
+      </c>
+      <c r="H127" s="10">
+        <v>5843804</v>
+      </c>
+      <c r="I127">
+        <v>23</v>
+      </c>
+      <c r="J127">
+        <v>55</v>
+      </c>
+      <c r="K127">
+        <v>1</v>
+      </c>
+      <c r="L127">
+        <v>1</v>
+      </c>
+      <c r="M127" s="42">
+        <v>2.89</v>
+      </c>
+      <c r="N127" s="42">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14">
+      <c r="A128" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B128" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D128" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E128" s="1">
+        <v>3</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G128" s="25">
+        <v>39989</v>
+      </c>
+      <c r="H128" s="10">
+        <v>6716122</v>
+      </c>
+      <c r="I128">
+        <v>23</v>
+      </c>
+      <c r="J128">
+        <v>55</v>
+      </c>
+      <c r="K128">
+        <v>1</v>
+      </c>
+      <c r="L128">
+        <v>1</v>
+      </c>
+      <c r="M128" s="42">
+        <v>2.93</v>
+      </c>
+      <c r="N128" s="42">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
+      <c r="A129" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="D129" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E129" s="1">
+        <v>4</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G129" s="25">
+        <v>39993</v>
+      </c>
+      <c r="H129" s="10">
+        <v>4325270</v>
+      </c>
+      <c r="I129">
+        <v>23</v>
+      </c>
+      <c r="J129">
+        <v>55</v>
+      </c>
+      <c r="K129">
+        <v>1</v>
+      </c>
+      <c r="L129">
+        <v>1</v>
+      </c>
+      <c r="M129" s="42">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="N129" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
+      <c r="A130" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B130" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D130" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G130" s="35">
+        <v>39954</v>
+      </c>
+      <c r="H130" s="10">
+        <v>5583407</v>
+      </c>
+      <c r="I130">
+        <v>23</v>
+      </c>
+      <c r="J130">
+        <v>55</v>
+      </c>
+      <c r="K130">
+        <v>1</v>
+      </c>
+      <c r="L130">
+        <v>1</v>
+      </c>
+      <c r="M130" s="42">
+        <v>2.15</v>
+      </c>
+      <c r="N130" s="43">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
+      <c r="A131" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B131" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D131" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E131" s="1">
+        <v>2</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G131" s="35">
+        <v>39960</v>
+      </c>
+      <c r="H131" s="10">
+        <v>3562441</v>
+      </c>
+      <c r="I131">
+        <v>23</v>
+      </c>
+      <c r="J131">
+        <v>55</v>
+      </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
+      <c r="L131">
+        <v>1</v>
+      </c>
+      <c r="M131" s="42">
+        <v>2.46</v>
+      </c>
+      <c r="N131" s="43">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
+      <c r="A132" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B132" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D132" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E132" s="1">
+        <v>3</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G132" s="35">
+        <v>39981</v>
+      </c>
+      <c r="H132" s="10">
+        <v>6401390</v>
+      </c>
+      <c r="I132">
+        <v>23</v>
+      </c>
+      <c r="J132">
+        <v>55</v>
+      </c>
+      <c r="K132">
+        <v>1</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="M132" s="42">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N132" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
+      <c r="A133" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B133" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D133" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E133" s="1">
+        <v>4</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G133" s="35">
+        <v>39982</v>
+      </c>
+      <c r="H133" s="10">
+        <v>7052258</v>
+      </c>
+      <c r="I133">
+        <v>23</v>
+      </c>
+      <c r="J133">
+        <v>55</v>
+      </c>
+      <c r="K133">
+        <v>1</v>
+      </c>
+      <c r="L133">
+        <v>1</v>
+      </c>
+      <c r="M133" s="42">
+        <v>2.31</v>
+      </c>
+      <c r="N133" s="42">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="A134" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B134" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C134" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D134" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="E134" s="1">
+        <v>1</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G134" s="23">
+        <v>39954</v>
+      </c>
+      <c r="H134" s="10">
+        <v>7862996</v>
+      </c>
+      <c r="I134">
+        <v>23</v>
+      </c>
+      <c r="J134">
+        <v>55</v>
+      </c>
+      <c r="K134">
+        <v>1</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
+      <c r="M134" s="42">
+        <v>2.88</v>
+      </c>
+      <c r="N134" s="43">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="A135" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B135" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C135" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="D135" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="E135" s="1">
+        <v>1</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G135" s="31">
+        <v>39967</v>
+      </c>
+      <c r="H135" s="10">
+        <v>8991527</v>
+      </c>
+      <c r="I135">
+        <v>23</v>
+      </c>
+      <c r="J135">
+        <v>55</v>
+      </c>
+      <c r="K135">
+        <v>1</v>
+      </c>
+      <c r="L135">
+        <v>1</v>
+      </c>
+      <c r="M135" s="42">
+        <v>2.33</v>
+      </c>
+      <c r="N135" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
+      <c r="A136" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C136" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="D136" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="E136" s="1">
+        <v>2</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G136" s="31">
+        <v>39989</v>
+      </c>
+      <c r="H136" s="10">
+        <v>5899707</v>
+      </c>
+      <c r="I136">
+        <v>23</v>
+      </c>
+      <c r="J136">
+        <v>55</v>
+      </c>
+      <c r="K136">
+        <v>1</v>
+      </c>
+      <c r="L136">
+        <v>1</v>
+      </c>
+      <c r="M136" s="42">
+        <v>2.98</v>
+      </c>
+      <c r="N136" s="42">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="A137" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B137" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="D137" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="E137" s="1">
+        <v>1</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G137" s="37">
+        <v>39960</v>
+      </c>
+      <c r="H137" s="10">
+        <v>2373866</v>
+      </c>
+      <c r="I137">
+        <v>23</v>
+      </c>
+      <c r="J137">
+        <v>55</v>
+      </c>
+      <c r="K137">
+        <v>1</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+      <c r="M137" s="42">
+        <v>2.69</v>
+      </c>
+      <c r="N137" s="43">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B138" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D138" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="E138" s="1">
+        <v>2</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G138" s="37">
+        <v>39993</v>
+      </c>
+      <c r="H138" s="10">
+        <v>4174779</v>
+      </c>
+      <c r="I138">
+        <v>23</v>
+      </c>
+      <c r="J138">
+        <v>55</v>
+      </c>
+      <c r="K138">
+        <v>1</v>
+      </c>
+      <c r="L138">
+        <v>1</v>
+      </c>
+      <c r="M138" s="42">
+        <v>1.86</v>
+      </c>
+      <c r="N138" s="42">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="A139" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B139" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D139" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E139" s="1">
+        <v>1</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" s="39">
+        <v>39968</v>
+      </c>
+      <c r="H139" s="10">
+        <v>5845429</v>
+      </c>
+      <c r="I139">
+        <v>23</v>
+      </c>
+      <c r="J139">
+        <v>55</v>
+      </c>
+      <c r="K139">
+        <v>1</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139" s="44">
+        <v>2.83</v>
+      </c>
+      <c r="N139" s="44">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B140" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D140" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E140" s="1">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G140" s="39">
+        <v>39968</v>
+      </c>
+      <c r="H140" s="10">
+        <v>5889335</v>
+      </c>
+      <c r="I140">
+        <v>23</v>
+      </c>
+      <c r="J140">
+        <v>55</v>
+      </c>
+      <c r="K140">
+        <v>1</v>
+      </c>
+      <c r="L140">
+        <v>1</v>
+      </c>
+      <c r="M140" s="43">
+        <v>2.83</v>
+      </c>
+      <c r="N140" s="43">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
+      <c r="A141" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B141" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D141" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E141" s="1">
+        <v>3</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G141" s="39">
+        <v>39986</v>
+      </c>
+      <c r="H141" s="10">
+        <v>6310775</v>
+      </c>
+      <c r="I141">
+        <v>23</v>
+      </c>
+      <c r="J141">
+        <v>55</v>
+      </c>
+      <c r="K141">
+        <v>1</v>
+      </c>
+      <c r="L141">
+        <v>1</v>
+      </c>
+      <c r="M141" s="42">
+        <v>3.07</v>
+      </c>
+      <c r="N141" s="42">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
+      <c r="A142" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B142" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C142" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D142" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E142" s="1">
+        <v>4</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G142" s="39">
+        <v>39988</v>
+      </c>
+      <c r="H142" s="10">
+        <v>6228121</v>
+      </c>
+      <c r="I142">
+        <v>23</v>
+      </c>
+      <c r="J142">
+        <v>55</v>
+      </c>
+      <c r="K142">
+        <v>1</v>
+      </c>
+      <c r="L142">
+        <v>1</v>
+      </c>
+      <c r="M142" s="42">
+        <v>2.59</v>
+      </c>
+      <c r="N142" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B143" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D143" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E143" s="1">
+        <v>1</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G143" s="41">
+        <v>39982</v>
+      </c>
+      <c r="H143" s="10">
+        <v>5926301</v>
+      </c>
+      <c r="I143">
+        <v>23</v>
+      </c>
+      <c r="J143">
+        <v>55</v>
+      </c>
+      <c r="K143">
+        <v>1</v>
+      </c>
+      <c r="L143">
+        <v>1</v>
+      </c>
+      <c r="M143" s="42">
+        <v>2.52</v>
+      </c>
+      <c r="N143" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="A144" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B144" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D144" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E144" s="1">
+        <v>2</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G144" s="41">
+        <v>39982</v>
+      </c>
+      <c r="H144" s="10">
+        <v>5902522</v>
+      </c>
+      <c r="I144">
+        <v>23</v>
+      </c>
+      <c r="J144">
+        <v>55</v>
+      </c>
+      <c r="K144">
+        <v>1</v>
+      </c>
+      <c r="L144">
+        <v>1</v>
+      </c>
+      <c r="M144" s="43">
+        <v>2.52</v>
+      </c>
+      <c r="N144" s="43">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B145" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C145" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D145" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E145" s="1">
+        <v>3</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G145" s="41">
+        <v>39993</v>
+      </c>
+      <c r="H145" s="10">
+        <v>4321734</v>
+      </c>
+      <c r="I145">
+        <v>23</v>
+      </c>
+      <c r="J145">
+        <v>55</v>
+      </c>
+      <c r="K145">
+        <v>1</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145" s="42">
+        <v>2.41</v>
+      </c>
+      <c r="N145" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B146" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="C146" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D146" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E146" s="1">
+        <v>4</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G146" s="41">
+        <v>39993</v>
+      </c>
+      <c r="H146" s="16">
+        <v>5049479</v>
+      </c>
+      <c r="I146">
+        <v>23</v>
+      </c>
+      <c r="J146">
+        <v>55</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+      <c r="M146" s="42">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="N146" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B147" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D147" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="E147" s="1">
+        <v>1</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G147" s="23">
+        <v>39965</v>
+      </c>
+      <c r="H147" s="10">
+        <v>8541404</v>
+      </c>
+      <c r="I147">
+        <v>23</v>
+      </c>
+      <c r="J147">
+        <v>55</v>
+      </c>
+      <c r="K147">
+        <v>1</v>
+      </c>
+      <c r="L147">
+        <v>1</v>
+      </c>
+      <c r="M147" s="42">
+        <v>2.59</v>
+      </c>
+      <c r="N147" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B148" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="C148" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D148" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E148" s="1">
+        <v>1</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G148" s="25">
+        <v>39982</v>
+      </c>
+      <c r="H148" s="10">
+        <v>7322238</v>
+      </c>
+      <c r="I148">
+        <v>23</v>
+      </c>
+      <c r="J148">
+        <v>55</v>
+      </c>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148" s="42">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="N148" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B149" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C149" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D149" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E149" s="1">
+        <v>2</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G149" s="25">
+        <v>39982</v>
+      </c>
+      <c r="H149" s="10">
+        <v>6880055</v>
+      </c>
+      <c r="I149">
+        <v>23</v>
+      </c>
+      <c r="J149">
+        <v>55</v>
+      </c>
+      <c r="K149">
+        <v>1</v>
+      </c>
+      <c r="L149">
+        <v>1</v>
+      </c>
+      <c r="M149" s="42">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="N149" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C150" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="D150" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E150" s="1">
+        <v>1</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G150" s="31">
+        <v>39960</v>
+      </c>
+      <c r="H150" s="10">
+        <v>3742005</v>
+      </c>
+      <c r="I150">
+        <v>23</v>
+      </c>
+      <c r="J150">
+        <v>55</v>
+      </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150" s="42">
+        <v>3.21</v>
+      </c>
+      <c r="N150" s="43">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B151" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="D151" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E151" s="1">
+        <v>2</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G151" s="31">
+        <v>39975</v>
+      </c>
+      <c r="H151" s="10">
+        <v>3043707</v>
+      </c>
+      <c r="I151">
+        <v>23</v>
+      </c>
+      <c r="J151">
+        <v>55</v>
+      </c>
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>1</v>
+      </c>
+      <c r="M151" s="42">
+        <v>3.63</v>
+      </c>
+      <c r="N151" s="42">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="A152" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B152" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D152" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E152" s="1">
+        <v>3</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G152" s="31">
+        <v>39981</v>
+      </c>
+      <c r="H152" s="10">
+        <v>5667215</v>
+      </c>
+      <c r="I152">
+        <v>23</v>
+      </c>
+      <c r="J152">
+        <v>55</v>
+      </c>
+      <c r="K152">
+        <v>1</v>
+      </c>
+      <c r="L152">
+        <v>1</v>
+      </c>
+      <c r="M152" s="42">
+        <v>3.97</v>
+      </c>
+      <c r="N152" s="42">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B153" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D153" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E153" s="1">
+        <v>4</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G153" s="31">
+        <v>39981</v>
+      </c>
+      <c r="H153" s="10">
+        <v>5508387</v>
+      </c>
+      <c r="I153">
+        <v>23</v>
+      </c>
+      <c r="J153">
+        <v>55</v>
+      </c>
+      <c r="K153">
+        <v>1</v>
+      </c>
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153" s="42">
+        <v>3.51</v>
+      </c>
+      <c r="N153" s="42">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B154" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C154" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="D154" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E154" s="1">
+        <v>5</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G154" s="31">
+        <v>39982</v>
+      </c>
+      <c r="H154" s="14">
+        <v>6364476</v>
+      </c>
+      <c r="I154">
+        <v>23</v>
+      </c>
+      <c r="J154">
+        <v>55</v>
+      </c>
+      <c r="K154">
+        <v>1</v>
+      </c>
+      <c r="L154">
+        <v>1</v>
+      </c>
+      <c r="M154" s="42">
+        <v>3.29</v>
+      </c>
+      <c r="N154" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="A155" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B155" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="C155" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="D155" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="E155" s="1">
+        <v>1</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G155" s="37">
+        <v>39968</v>
+      </c>
+      <c r="H155" s="10">
+        <v>7088155</v>
+      </c>
+      <c r="I155">
+        <v>23</v>
+      </c>
+      <c r="J155">
+        <v>55</v>
+      </c>
+      <c r="K155">
+        <v>1</v>
+      </c>
+      <c r="L155">
+        <v>1</v>
+      </c>
+      <c r="M155" s="43">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N155" s="43">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B156" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="D156" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="E156" s="1">
+        <v>2</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G156" s="37">
+        <v>39986</v>
+      </c>
+      <c r="H156" s="10">
+        <v>5652562</v>
+      </c>
+      <c r="I156">
+        <v>23</v>
+      </c>
+      <c r="J156">
+        <v>55</v>
+      </c>
+      <c r="K156">
+        <v>1</v>
+      </c>
+      <c r="L156">
+        <v>1</v>
+      </c>
+      <c r="M156" s="42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N156" s="42">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B157" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="C157" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="D157" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="E157" s="1">
+        <v>1</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G157" s="23">
+        <v>39986</v>
+      </c>
+      <c r="H157" s="10">
+        <v>6837468</v>
+      </c>
+      <c r="I157">
+        <v>23</v>
+      </c>
+      <c r="J157">
+        <v>55</v>
+      </c>
+      <c r="K157">
+        <v>1</v>
+      </c>
+      <c r="L157">
+        <v>1</v>
+      </c>
+      <c r="M157" s="42">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N157" s="42">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="A158" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B158" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C158" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D158" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="E158" s="1">
+        <v>1</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G158" s="41">
+        <v>39968</v>
+      </c>
+      <c r="H158" s="10">
+        <v>6333090</v>
+      </c>
+      <c r="I158">
+        <v>23</v>
+      </c>
+      <c r="J158">
+        <v>55</v>
+      </c>
+      <c r="K158">
+        <v>1</v>
+      </c>
+      <c r="L158">
+        <v>1</v>
+      </c>
+      <c r="M158" s="43">
+        <v>2.16</v>
+      </c>
+      <c r="N158" s="43">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="A159" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B159" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C159" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="D159" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="E159" s="1">
+        <v>2</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G159" s="41">
+        <v>39986</v>
+      </c>
+      <c r="H159" s="10">
+        <v>6828056</v>
+      </c>
+      <c r="I159">
+        <v>23</v>
+      </c>
+      <c r="J159">
+        <v>55</v>
+      </c>
+      <c r="K159">
+        <v>1</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
+      <c r="M159" s="43">
+        <v>2.16</v>
+      </c>
+      <c r="N159" s="43">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B160" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C160" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="D160" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="E160" s="1">
+        <v>3</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G160" s="41">
+        <v>39989</v>
+      </c>
+      <c r="H160" s="10">
+        <v>6376735</v>
+      </c>
+      <c r="I160">
+        <v>23</v>
+      </c>
+      <c r="J160">
+        <v>55</v>
+      </c>
+      <c r="K160">
+        <v>1</v>
+      </c>
+      <c r="L160">
+        <v>1</v>
+      </c>
+      <c r="M160" s="42">
+        <v>2.16</v>
+      </c>
+      <c r="N160" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14">
+      <c r="A161" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B161" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C161" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="D161" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E161" s="1">
+        <v>1</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G161" s="37">
+        <v>39973</v>
+      </c>
+      <c r="H161" s="16">
+        <v>6351713</v>
+      </c>
+      <c r="I161">
+        <v>23</v>
+      </c>
+      <c r="J161">
+        <v>55</v>
+      </c>
+      <c r="K161">
+        <v>1</v>
+      </c>
+      <c r="L161">
+        <v>1</v>
+      </c>
+      <c r="M161" s="42">
+        <v>2.54</v>
+      </c>
+      <c r="N161" s="42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B162" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C162" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D162" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E162" s="1">
+        <v>2</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G162" s="37">
+        <v>39975</v>
+      </c>
+      <c r="H162" s="10">
+        <v>3672661</v>
+      </c>
+      <c r="I162">
+        <v>23</v>
+      </c>
+      <c r="J162">
+        <v>55</v>
+      </c>
+      <c r="K162">
+        <v>1</v>
+      </c>
+      <c r="L162">
+        <v>1</v>
+      </c>
+      <c r="M162" s="42">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="N162" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14">
+      <c r="A163" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B163" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C163" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="D163" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E163" s="1">
+        <v>3</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G163" s="37">
+        <v>39981</v>
+      </c>
+      <c r="H163" s="10">
+        <v>4164637</v>
+      </c>
+      <c r="I163">
+        <v>23</v>
+      </c>
+      <c r="J163">
+        <v>55</v>
+      </c>
+      <c r="K163">
+        <v>1</v>
+      </c>
+      <c r="L163">
+        <v>1</v>
+      </c>
+      <c r="M163" s="42">
+        <v>2.88</v>
+      </c>
+      <c r="N163" s="42">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="A164" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B164" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C164" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D164" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E164" s="1">
+        <v>4</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G164" s="37">
+        <v>39982</v>
+      </c>
+      <c r="H164" s="10">
+        <v>5507287</v>
+      </c>
+      <c r="I164">
+        <v>23</v>
+      </c>
+      <c r="J164">
+        <v>55</v>
+      </c>
+      <c r="K164">
+        <v>1</v>
+      </c>
+      <c r="L164">
+        <v>1</v>
+      </c>
+      <c r="M164" s="42">
+        <v>3.05</v>
+      </c>
+      <c r="N164" s="42">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="A165" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B165" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="D165" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E165" s="1">
+        <v>5</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G165" s="37">
+        <v>39982</v>
+      </c>
+      <c r="H165" s="10">
+        <v>5509231</v>
+      </c>
+      <c r="I165">
+        <v>23</v>
+      </c>
+      <c r="J165">
+        <v>55</v>
+      </c>
+      <c r="K165">
+        <v>1</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165" s="42">
+        <v>3.05</v>
+      </c>
+      <c r="N165" s="42">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B166" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C166" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="D166" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E166" s="1">
+        <v>6</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G166" s="37">
+        <v>39989</v>
+      </c>
+      <c r="H166" s="10">
+        <v>7714599</v>
+      </c>
+      <c r="I166">
+        <v>23</v>
+      </c>
+      <c r="J166">
+        <v>55</v>
+      </c>
+      <c r="K166">
+        <v>1</v>
+      </c>
+      <c r="L166">
+        <v>1</v>
+      </c>
+      <c r="M166" s="42">
+        <v>3.15</v>
+      </c>
+      <c r="N166" s="42">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14">
+      <c r="A167" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B167" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C167" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="D167" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E167" s="1">
+        <v>7</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G167" s="37">
+        <v>39989</v>
+      </c>
+      <c r="H167" s="10">
+        <v>7684939</v>
+      </c>
+      <c r="I167">
+        <v>23</v>
+      </c>
+      <c r="J167">
+        <v>55</v>
+      </c>
+      <c r="K167">
+        <v>1</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="M167" s="43">
+        <v>3.15</v>
+      </c>
+      <c r="N167" s="43">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14">
+      <c r="A168" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B168" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C168" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="D168" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E168" s="1">
+        <v>8</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G168" s="37">
+        <v>39993</v>
+      </c>
+      <c r="H168" s="10">
+        <v>5524166</v>
+      </c>
+      <c r="I168">
+        <v>23</v>
+      </c>
+      <c r="J168">
+        <v>55</v>
+      </c>
+      <c r="K168">
+        <v>1</v>
+      </c>
+      <c r="L168">
+        <v>1</v>
+      </c>
+      <c r="M168" s="44">
+        <v>2.89</v>
+      </c>
+      <c r="N168" s="44">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B169" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="C169" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D169" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E169" s="1">
+        <v>1</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G169" s="25">
+        <v>39986</v>
+      </c>
+      <c r="H169" s="10">
+        <v>6133306</v>
+      </c>
+      <c r="I169">
+        <v>23</v>
+      </c>
+      <c r="J169">
+        <v>55</v>
+      </c>
+      <c r="K169">
+        <v>1</v>
+      </c>
+      <c r="L169">
+        <v>1</v>
+      </c>
+      <c r="M169" s="42">
+        <v>2.68</v>
+      </c>
+      <c r="N169" s="42">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B170" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="C170" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E170" s="1">
+        <v>2</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G170" s="25">
+        <v>39986</v>
+      </c>
+      <c r="H170" s="10">
+        <v>6120525</v>
+      </c>
+      <c r="I170">
+        <v>23</v>
+      </c>
+      <c r="J170">
+        <v>55</v>
+      </c>
+      <c r="K170">
+        <v>1</v>
+      </c>
+      <c r="L170">
+        <v>1</v>
+      </c>
+      <c r="M170" s="43">
+        <v>2.68</v>
+      </c>
+      <c r="N170" s="43">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14">
+      <c r="A171" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B171" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="C171" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="D171" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E171" s="1">
+        <v>3</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G171" s="25">
+        <v>39993</v>
+      </c>
+      <c r="H171" s="15">
+        <v>5619639</v>
+      </c>
+      <c r="I171">
+        <v>23</v>
+      </c>
+      <c r="J171">
+        <v>55</v>
+      </c>
+      <c r="K171">
+        <v>1</v>
+      </c>
+      <c r="L171">
+        <v>1</v>
+      </c>
+      <c r="M171" s="42">
+        <v>2.78</v>
+      </c>
+      <c r="N171" s="42">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>